<commit_message>
plus product added to the list
</commit_message>
<xml_diff>
--- a/PositionInfo/full_Port_v2.xlsx
+++ b/PositionInfo/full_Port_v2.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="366">
   <si>
     <t>Name</t>
   </si>
@@ -1136,6 +1136,24 @@
   </si>
   <si>
     <t>Rakuten</t>
+  </si>
+  <si>
+    <t>Elixinol Global Ltd</t>
+  </si>
+  <si>
+    <t>Elixinol</t>
+  </si>
+  <si>
+    <t>ELLXF</t>
+  </si>
+  <si>
+    <t>Plus Product</t>
+  </si>
+  <si>
+    <t>Plus Product Inc</t>
+  </si>
+  <si>
+    <t>PLPRF</t>
   </si>
 </sst>
 </file>
@@ -1482,6 +1500,26 @@
   <dxfs count="21">
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1765,26 +1803,6 @@
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
@@ -20023,17 +20041,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="RiskTab22" displayName="RiskTab22" ref="A1:I95" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="RiskTab22" displayName="RiskTab22" ref="A1:I97" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19">
   <tableColumns count="9">
-    <tableColumn id="1" name="Nr." dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="12" name="Category" totalsRowDxfId="13"/>
-    <tableColumn id="9" name="ShortName" totalsRowDxfId="12"/>
-    <tableColumn id="24" name="Name" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="5" name="Volume" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="32" name="AlphaVantage" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="3" name="ISIN" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="4" name="WKN" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="2" name="FT" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="1" name="Nr." dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="12" name="Category" totalsRowDxfId="15"/>
+    <tableColumn id="9" name="ShortName" totalsRowDxfId="14"/>
+    <tableColumn id="24" name="Name" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="5" name="Volume" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="32" name="AlphaVantage" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="3" name="ISIN" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="4" name="WKN" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="2" name="FT" dataDxfId="3" totalsRowDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -20326,13 +20344,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I95"/>
+  <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="H56" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H71" sqref="H71"/>
+      <selection pane="bottomRight" activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -22489,46 +22507,46 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>291</v>
+        <v>262</v>
       </c>
       <c r="C83" t="s">
-        <v>302</v>
+        <v>361</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="E83" s="11" t="s">
-        <v>315</v>
-      </c>
+        <v>360</v>
+      </c>
+      <c r="E83" s="10"/>
       <c r="F83" s="1" t="s">
-        <v>303</v>
+        <v>362</v>
       </c>
       <c r="G83" s="7"/>
       <c r="H83" s="7"/>
-      <c r="I83" s="7" t="s">
-        <v>315</v>
-      </c>
+      <c r="I83" s="14"/>
     </row>
     <row r="84" spans="1:9">
       <c r="A84">
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>328</v>
+        <v>291</v>
       </c>
       <c r="C84" t="s">
-        <v>327</v>
+        <v>302</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>327</v>
-      </c>
-      <c r="E84" s="13"/>
+        <v>301</v>
+      </c>
+      <c r="E84" s="11" t="s">
+        <v>315</v>
+      </c>
       <c r="F84" s="1" t="s">
-        <v>326</v>
+        <v>303</v>
       </c>
       <c r="G84" s="7"/>
       <c r="H84" s="7"/>
-      <c r="I84" s="14"/>
+      <c r="I84" s="7" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="85" spans="1:9">
       <c r="A85">
@@ -22538,14 +22556,14 @@
         <v>328</v>
       </c>
       <c r="C85" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D85" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E85" s="13"/>
       <c r="F85" s="1" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="G85" s="7"/>
       <c r="H85" s="7"/>
@@ -22559,14 +22577,14 @@
         <v>328</v>
       </c>
       <c r="C86" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E86" s="13"/>
       <c r="F86" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="G86" s="7"/>
       <c r="H86" s="7"/>
@@ -22577,17 +22595,17 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="C87" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D87" s="11" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="E87" s="13"/>
       <c r="F87" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="G87" s="7"/>
       <c r="H87" s="7"/>
@@ -22601,20 +22619,20 @@
         <v>335</v>
       </c>
       <c r="C88" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="D88" s="11" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E88" s="13"/>
       <c r="F88" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="G88" s="7"/>
       <c r="H88" s="7"/>
       <c r="I88" s="14"/>
     </row>
-    <row r="89" spans="1:9" ht="15" customHeight="1">
+    <row r="89" spans="1:9">
       <c r="A89">
         <v>88</v>
       </c>
@@ -22622,20 +22640,20 @@
         <v>335</v>
       </c>
       <c r="C89" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E89" s="13"/>
       <c r="F89" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="G89" s="7"/>
       <c r="H89" s="7"/>
       <c r="I89" s="14"/>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" ht="15" customHeight="1">
       <c r="A90">
         <v>89</v>
       </c>
@@ -22643,14 +22661,14 @@
         <v>335</v>
       </c>
       <c r="C90" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="D90" s="11" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="E90" s="13"/>
       <c r="F90" s="1" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="G90" s="7"/>
       <c r="H90" s="7"/>
@@ -22664,14 +22682,14 @@
         <v>335</v>
       </c>
       <c r="C91" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="D91" s="11" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="E91" s="13"/>
       <c r="F91" s="1" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="G91" s="7"/>
       <c r="H91" s="7"/>
@@ -22685,14 +22703,14 @@
         <v>335</v>
       </c>
       <c r="C92" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="D92" s="11" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="E92" s="13"/>
       <c r="F92" s="1" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="G92" s="7"/>
       <c r="H92" s="7"/>
@@ -22706,14 +22724,14 @@
         <v>335</v>
       </c>
       <c r="C93" t="s">
-        <v>349</v>
+        <v>359</v>
       </c>
       <c r="D93" s="11" t="s">
-        <v>348</v>
+        <v>358</v>
       </c>
       <c r="E93" s="13"/>
       <c r="F93" s="1" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="G93" s="7"/>
       <c r="H93" s="7"/>
@@ -22724,59 +22742,101 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>291</v>
+        <v>335</v>
       </c>
       <c r="C94" t="s">
-        <v>299</v>
-      </c>
-      <c r="D94" t="s">
-        <v>298</v>
-      </c>
-      <c r="E94" t="s">
-        <v>315</v>
-      </c>
+        <v>349</v>
+      </c>
+      <c r="D94" s="11" t="s">
+        <v>348</v>
+      </c>
+      <c r="E94" s="13"/>
       <c r="F94" s="1" t="s">
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="G94" s="7"/>
       <c r="H94" s="7"/>
-      <c r="I94" s="7" t="s">
-        <v>315</v>
-      </c>
+      <c r="I94" s="14"/>
     </row>
     <row r="95" spans="1:9">
       <c r="A95">
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>324</v>
+        <v>262</v>
       </c>
       <c r="C95" t="s">
-        <v>323</v>
-      </c>
-      <c r="D95" t="s">
-        <v>323</v>
-      </c>
-      <c r="E95" t="s">
-        <v>315</v>
-      </c>
+        <v>363</v>
+      </c>
+      <c r="D95" s="11" t="s">
+        <v>364</v>
+      </c>
+      <c r="E95" s="13"/>
       <c r="F95" s="1" t="s">
-        <v>325</v>
+        <v>365</v>
       </c>
       <c r="G95" s="7"/>
       <c r="H95" s="7"/>
-      <c r="I95" s="7" t="s">
+      <c r="I95" s="14"/>
+    </row>
+    <row r="96" spans="1:9">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>291</v>
+      </c>
+      <c r="C96" t="s">
+        <v>299</v>
+      </c>
+      <c r="D96" t="s">
+        <v>298</v>
+      </c>
+      <c r="E96" t="s">
+        <v>315</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="G96" s="7"/>
+      <c r="H96" s="7"/>
+      <c r="I96" s="7" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>324</v>
+      </c>
+      <c r="C97" t="s">
+        <v>323</v>
+      </c>
+      <c r="D97" t="s">
+        <v>323</v>
+      </c>
+      <c r="E97" t="s">
+        <v>315</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="G97" s="7"/>
+      <c r="H97" s="7"/>
+      <c r="I97" s="7" t="s">
         <v>315</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D38:E55 D2:E36">
-    <cfRule type="expression" dxfId="20" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>#REF!=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37:E37">
-    <cfRule type="expression" dxfId="19" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>#REF!=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>